<commit_message>
with out iframes check
</commit_message>
<xml_diff>
--- a/randomfeed.xlsx
+++ b/randomfeed.xlsx
@@ -14,120 +14,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
-  <si>
-    <t>http://amazon.co.uk</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="53">
+  <si>
+    <t>http://upwork.com/login</t>
+  </si>
+  <si>
+    <t>the webpage is Phishing based on URLHeuristic score</t>
+  </si>
+  <si>
+    <t>http://i.yiche.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the webpage is phish as pwd field is not in second page </t>
   </si>
   <si>
     <t>no password field in start page</t>
   </si>
   <si>
-    <t>http://aliexpress.com/</t>
+    <t>http://zoho.com</t>
+  </si>
+  <si>
+    <t>second page based genuine website &amp; URL Heuristic score is != 1</t>
+  </si>
+  <si>
+    <t>http://engadget.com</t>
+  </si>
+  <si>
+    <t>http://engadget.com/user/login/</t>
+  </si>
+  <si>
+    <t>http://signin.ebay.in/ws/eBayISAPI.dll?SignIn&amp;ru=http%3A%2F%2Fwww.ebay.in%2F</t>
+  </si>
+  <si>
+    <t>http://ancestry.com/</t>
+  </si>
+  <si>
+    <t>http://login.oracle.com/mysso/signon.jsp</t>
+  </si>
+  <si>
+    <t>http://blogfa.com/</t>
+  </si>
+  <si>
+    <t>the webpage is Phishing based on successful logging in second page</t>
+  </si>
+  <si>
+    <t>http://online.citi.com/US/Welcome.c</t>
   </si>
   <si>
     <t>http://login.yahoo.com/config/login?.src=flickrsignin&amp;.pc=8190&amp;.scrumb=0&amp;.pd=c%3DH6T9XcS72e4mRnW3NpTAiU8ZkA--&amp;.intl=in&amp;.lang=en&amp;mg=1&amp;.done=https%3A%2F%2Flogin.yahoo.com%2Fconfig%2Fvalidate%3F.src%3Dflickrsignin%26.pc%3D8190%26.scrumb%3D0%26.pd%3Dc%253DJvVF95K62e6PzdPu7MBv2V8-%26.intl%3Din%26.done%3Dhttps%253A%252F%252Fwww.flickr.com%252Fsignin%252Fyahoo%252F%253Fredir%253Dhttps%25253A%25252F%25252Fwww.flickr.com%25252F</t>
   </si>
   <si>
-    <t>http://rakuten.co.jp</t>
-  </si>
-  <si>
-    <t>http://cntv.cn</t>
-  </si>
-  <si>
-    <t>http://coccoc.com</t>
-  </si>
-  <si>
-    <t>http://google.com.tw</t>
-  </si>
-  <si>
-    <t>http://popads.net</t>
-  </si>
-  <si>
-    <t>the webpage is Phishing based on URLHeuristic score</t>
-  </si>
-  <si>
-    <t>http://microsoftonline.com</t>
-  </si>
-  <si>
-    <t>second page based genuine website &amp; URL Heuristic score is != 1</t>
-  </si>
-  <si>
-    <t>http://bongacams.com</t>
-  </si>
-  <si>
-    <t>http://wikia.com</t>
-  </si>
-  <si>
-    <t>http://twitch.tv</t>
-  </si>
-  <si>
-    <t>http://cnn.com</t>
-  </si>
-  <si>
-    <t>http://google.com.eg</t>
-  </si>
-  <si>
-    <t>http://booking.com</t>
-  </si>
-  <si>
-    <t>http://haosou.com</t>
-  </si>
-  <si>
-    <t>http://bbc.co.uk</t>
-  </si>
-  <si>
-    <t>http://adobe.com</t>
-  </si>
-  <si>
-    <t>http://google.com.pk</t>
-  </si>
-  <si>
-    <t>http://google.com.sa</t>
-  </si>
-  <si>
-    <t>http://chase.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the webpage is phish as pwd field is not in second page </t>
-  </si>
-  <si>
-    <t>http://daum.net</t>
-  </si>
-  <si>
-    <t>http://flipkart.com</t>
-  </si>
-  <si>
-    <t>http://163.com</t>
-  </si>
-  <si>
-    <t>http://google.co.th</t>
-  </si>
-  <si>
-    <t>http://alipay.com</t>
-  </si>
-  <si>
-    <t>http://china.com</t>
-  </si>
-  <si>
-    <t>http://espn.go.com</t>
-  </si>
-  <si>
-    <t>http://sogou.com</t>
-  </si>
-  <si>
-    <t>http://nytimes.com</t>
-  </si>
-  <si>
-    <t>http://bilibili.com</t>
-  </si>
-  <si>
-    <t>http://ebay.de</t>
-  </si>
-  <si>
-    <t>http://bbc.com</t>
-  </si>
-  <si>
-    <t>http://ettoday.net</t>
+    <t>http://pinterest.com/</t>
+  </si>
+  <si>
+    <t>http://i.huanqiu.com/register</t>
+  </si>
+  <si>
+    <t>http://amazon.es/ap/signin?_encoding=UTF8&amp;openid.assoc_handle=esflex&amp;openid.claimed_id=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0%2Fidentifier_select&amp;openid.identity=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0%2Fidentifier_select&amp;openid.mode=checkid_setup&amp;openid.ns=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0&amp;openid.ns.pape=http%3A%2F%2Fspecs.openid.net%2Fextensions%2Fpape%2F1.0&amp;openid.pape.max_auth_age=0&amp;openid.return_to=https%3A%2F%2Fwww.amazon.es%2F276-9212693-4729315%3Fref_%3Dnav_signin</t>
+  </si>
+  <si>
+    <t>http://sourceforge.net/auth/</t>
+  </si>
+  <si>
+    <t>http://americanexpress.com/in/</t>
+  </si>
+  <si>
+    <t>http://ssl.allegro.pl/login/form?authorization_uri=https:%2F%2Fssl.allegro.pl%2Fauth%2Foauth%2Fauthorize%3Fclient_id%3Dtb5SFf3cRxEyspDN%26redirect_uri%3Dhttps:%2F%2Fssl.allegro.pl%2Flogin%2Fauth%3Forigin_url%253Dhttp%25253A%25252F%25252Fallegro.pl%25252F%2526qstate%253DeyJndWVzdCI6W10sInJlcXVlc3QiOiIiLCJ1cmxQcmVmaXgiOiJodHRwOlwvXC9hbGxlZ3JvLnBsXC8iLCJjb2JyYW5kSWQiOjAsInRva2VuIjoiMTJjN2E1ZWQ2MmRlNTQ0Y2Q5ZGJhYzdkNzQwMjFiZGMiLCJmYWNlYm9va0FjY2Vzc1Rva2VuIjpudWxsfQ%25253D%25253D%26response_type%3Dcode%26state%3De5IL6K&amp;oauth=true</t>
+  </si>
+  <si>
+    <t>http://login.live.com/login.srf?wa=wsignin1.0&amp;rpsnv=12&amp;ct=1464355433&amp;rver=6.7.6643.0&amp;wp=MBI_SSL&amp;wreply=https%3A%2F%2Fstores.office.com%2Fauthredir%3Furl%3Dhttps%253a%252f%252fstores.office.com%253a443%252fmyaccount%252fhome.aspx%253fui%253den-US%2526rs%253den-US%2526ad%253dUS%26hurl%3DHNRMIT1%252fp07QH9wDV49zqR4PjxAIoOCnPqoeBaMLC3Q%253d.yVzA1JrJwl83JnmlLA5LBMcR2Hxkcnj3DWZe14p9ErY%253d%26ipt%3D0&amp;lc=1033&amp;id=290950&amp;lw=1&amp;fl=easi2&amp;cobrandid=90012</t>
+  </si>
+  <si>
+    <t>http://att.com/olam/loginAction.olamexecute?source=IC4425j4900s2000</t>
+  </si>
+  <si>
+    <t>http://sbi.sberbank.ru:9443/ic/login.zhtml</t>
+  </si>
+  <si>
+    <t>http://passport.1905.com/v2/?m=user&amp;a=login&amp;callback_url=http%3A%2F%2Fwww.1905.com%2F</t>
+  </si>
+  <si>
+    <t>http://um.mama.cn/passport/?key=tianjing&amp;service=http%3A%2F%2Fwww.mama.cn%2F%3Fg%3DHome%26a%3DPassport%26d%3DgetUserInfo%26callback%3Dcheckcallback%26code%3D3c904cf3e4664db2bdc0d90d092a7900%26i%3D177893%26_%3D1430360903204&amp;t=1430364752&amp;sign=38f108855efb02ca255b13bcd8b8090a</t>
+  </si>
+  <si>
+    <t>http://goodreads.com/</t>
+  </si>
+  <si>
+    <t>http://accounts.tokopedia.com/authorize?response_type=code&amp;client_id=1001&amp;state=eyJyZWYiOiJodHRwczovL3d3dy50b2tvcGVkaWEuY29tLyIsInV1aWQiOiI5MzM4NzgxYi1iOTI1LTQ2MTgtYWYyYi00ZjdjMDc3OTk3MTUiLCJ0aGVtZSI6ImRlZmF1bHQifQ&amp;redirect_uri=https%3A%2F%2Faccounts.tokopedia.com%2Fappauth%2Fcode&amp;p=https://www.tokopedia.com&amp;contactus=&amp;theme=default</t>
+  </si>
+  <si>
+    <t>http://banking.capitalone.com/</t>
+  </si>
+  <si>
+    <t>http://weebly.com/#login</t>
+  </si>
+  <si>
+    <t>http://popcash.net/members/login</t>
+  </si>
+  <si>
+    <t>http://auth.telegraph.co.uk/sam-ui/login.htm;jsessionid=C843D3C24C1C3D60FCAEC9DE84C6DEE5.jvmfe2dr?logintype=tmg&amp;redirectTo=http%3A%2F%2Fwww.telegraph.co.uk%2F&amp;logoFilename=&amp;title=Log+in+to+your+Telegraph+profile&amp;skinFooterImage=%2Fsam-ui%2Fi%2Ftcuk-footer-logo.gif&amp;description=You+need+to+register+to+access+certain+parts+of+our+site.+You+will+be+able+to+sign+up+for+free%0A++++++++++++email+bulletins+and+take+part+in+competitions.%0A++++++++&amp;skinCss=%2Fsam-ui%2Fcss-</t>
+  </si>
+  <si>
+    <t>http://infinity.icicibank.com/corp/AuthenticationController?FORMSGROUP_ID__=AuthenticationFG&amp;__START_TRAN_FLAG__=Y&amp;FG_BUTTONS__=LOAD&amp;ACTION.LOAD=Y&amp;AuthenticationFG.LOGIN_FLAG=1&amp;BANK_ID=ICI</t>
+  </si>
+  <si>
+    <t>http://auth.telegraph.co.uk/sam-ui/login.htm;jsessionid=C843D3C24C1C3D60FCAEC9DE84C6DEE5.jvmfe2dr?logintype=tmg&amp;redirectTo=http%3A%2F%2Fwww.telegraph.co.uk%2F&amp;logoFilename=&amp;title=Log+in+to+your+Telegraph+profile&amp;skinFooterImage=%2Fsam-ui%2Fi%2Ftcuk-footer-logo.gif&amp;description=You+need+to+register+to+access+certain+parts+of+our+site.+You+will+be+able+to+sign+up+for+free%0A++++++++++++email+bulletins+and+take+part+in+competitions.%0A++++++++&amp;skinCss=%2Fsam-ui%2Fcss-v3%2Fdigital.css&amp;skinImageAlt=Telegraph.co.uk&amp;skinImage=%2Fsam-ui%2Fi-v3%2FtmgLogo.gif</t>
+  </si>
+  <si>
+    <t>http://reg.usps.com/entreg/LoginAction_input?app=Phoenix&amp;appURL=https://www.usps.com/</t>
+  </si>
+  <si>
+    <t>http://https://cib.icicibank.com/corp/BANKAWAY?Action.CorpUser.Init1.001=Y&amp;AppSignonBankId=ICI&amp;AppType=corporate</t>
+  </si>
+  <si>
+    <t>http://cib.icicibank.com/corp/BANKAWAY?Action.CorpUser.Init1.001=Y&amp;AppSignonBankId=ICI&amp;AppType=corporate</t>
+  </si>
+  <si>
+    <t>http://infinity.icicibank.com/corp/Login.jsp</t>
+  </si>
+  <si>
+    <t>http://blastingnews.com/</t>
+  </si>
+  <si>
+    <t>http://subscribe.washingtonpost.com/loginregistration/index.html#/register/group/long?action=login&amp;destination=https:%2F%2Fwww.washingtonpost.com%2F</t>
+  </si>
+  <si>
+    <t>http://zhihu.com/</t>
+  </si>
+  <si>
+    <t>http://stackexchange.com/users/login?returnurl=http%3a%2f%2fstackexchange.com%2f#log-in</t>
+  </si>
+  <si>
+    <t>http://accounts.pixiv.net/login?lang=en&amp;source=pc&amp;view_type=page&amp;ref=wwwtop_accounts_index</t>
+  </si>
+  <si>
+    <t>http://adobeid-na1.services.adobe.com/renga-idprovider/pages/login?callback=https%3A%2F%2Fims-na1.adobelogin.com%2Fims%2Fadobeid%2Fadobedotcom2%2FAdobeID%2Ftoken%3Fredirect_uri%3Dhttps%253A%252F%252Fwww.adobe.com%252F%2523from_ims%253Dtrue%2526old_hash%253D%252523%2526api%253Dauthorize&amp;client_id=adobedotcom2&amp;scope=creative_cloud%2CAdobeID%2Copenid%2Cgnav%2Cread_organizations%2Cadditional_info.projectedProductContext%2Csao.ACOM_CLOUD_STORAGE%2Csao.stock%2Csao.cce_private%2Cadditional_info.roles&amp;display=web_v2&amp;denied_callback=https%3A%2F%2Fims-</t>
+  </si>
+  <si>
+    <t>http://walmart.com/account/login</t>
+  </si>
+  <si>
+    <t>http://vimeo.com/</t>
+  </si>
+  <si>
+    <t>http://weather.com/</t>
+  </si>
+  <si>
+    <t>http://ssl.bbc.com/id/signin?ptrt=http%3A%2F%2Fwww.bbc.com%2F</t>
+  </si>
+  <si>
+    <t>http://popads.net/</t>
+  </si>
+  <si>
+    <t>http://zillow.com/</t>
+  </si>
+  <si>
+    <t>http://english.cntv.cn/include/ztbhy/login/index.shtml#backurl=http://english.cctv.com/</t>
+  </si>
+  <si>
+    <t>http://login.alibaba.com/?spm=a2700.7848340.a2728m.1.6dwgtQ</t>
   </si>
 </sst>
 </file>
@@ -473,177 +518,57 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="A1:B19"/>
+      <selection activeCell="I13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>